<commit_message>
added new footer xpath
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Product" sheetId="2" r:id="rId3"/>
     <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
     <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>パスワード</t>
   </si>
@@ -87,6 +86,34 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>クレジットカード番号</t>
+  </si>
+  <si>
+    <t>有効期限（月）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">有効期限（年）
+</t>
+  </si>
+  <si>
+    <t>カード名義</t>
+  </si>
+  <si>
+    <t>セキュリティコード</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
   <si>
     <t>Test Card</t>
@@ -136,53 +163,10 @@
     <t>spoan.patil@scispl.com</t>
   </si>
   <si>
+    <t>Failure</t>
+  </si>
+  <si>
     <t>sopan181</t>
-  </si>
-  <si>
-    <t>2月</t>
-  </si>
-  <si>
-    <t>1111111111111111</t>
-  </si>
-  <si>
-    <t>E61: E61010002: カードの登録に失敗しました</t>
-  </si>
-  <si>
-    <t>飯田</t>
-  </si>
-  <si>
-    <t>弘明</t>
-  </si>
-  <si>
-    <t>イイダ</t>
-  </si>
-  <si>
-    <t>ヒロアキ</t>
-  </si>
-  <si>
-    <t>女</t>
-  </si>
-  <si>
-    <t>2006 (平成18年)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">兵庫県
-                                    </t>
-  </si>
-  <si>
-    <t>犬上郡多賀町</t>
-  </si>
-  <si>
-    <t>中川原</t>
-  </si>
-  <si>
-    <t>新屋敷アパート</t>
-  </si>
-  <si>
-    <t>輝夜ホーム</t>
-  </si>
-  <si>
-    <t>075</t>
   </si>
 </sst>
 </file>
@@ -240,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -262,15 +246,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -590,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +578,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -758,41 +733,91 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>33</v>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4111111111111110</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1">
         <v>2025</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2">
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2">
         <v>1213</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4111111111111110</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2025</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1213</v>
       </c>
     </row>
   </sheetData>
@@ -823,90 +848,90 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
         <v>749690140</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1">
         <v>749690140</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1">
         <v>749690140</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1">
         <v>749690140</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -917,86 +942,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="9" style="1"/>
-    <col min="13" max="13" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" style="11"/>
-    <col min="17" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1">
-        <v>503</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2313</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>9695</v>
-      </c>
-      <c r="R1" s="1">
-        <v>1140</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'main' into Sopan_MyPage_PT_45_49"
This reverts commit 20361a297fc4806c02efde332259214b90f97b5c, reversing
changes made to b231caab9e2df7092ce7980dd6466da350bb67a0.
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\WorkSpace\Project\Workspace\GitPFAutomation\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sopan\Project\Automation\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20734" windowHeight="11160" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
     <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
     <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="NewUser" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>パスワード</t>
   </si>
@@ -174,15 +173,6 @@
   </si>
   <si>
     <t>075</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>EID</t>
   </si>
 </sst>
 </file>
@@ -594,14 +584,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.3828125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -625,12 +615,12 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -716,14 +706,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.3828125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -732,7 +722,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -741,7 +731,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -764,18 +754,18 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.3046875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.53515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.84375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -809,19 +799,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.15234375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.53515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.84375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
@@ -839,7 +829,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -858,7 +848,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -875,7 +865,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -892,7 +882,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
@@ -923,21 +913,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="14.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="11"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -982,30 +972,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added new data to excel
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>パスワード</t>
   </si>
@@ -181,10 +181,13 @@
     <t>EID</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>email2</t>
+    <t>TestPF1221+05082021123419@gmail.com</t>
+  </si>
+  <si>
+    <t>pfqa_123</t>
+  </si>
+  <si>
+    <t>TestPF1221_05082021123419</t>
   </si>
 </sst>
 </file>
@@ -992,10 +995,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="17.3046875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.84375" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
@@ -1010,7 +1017,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
New user validated with login
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="2" windowHeight="3343" windowWidth="18120" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="3343" windowWidth="18120" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="User" r:id="rId1" sheetId="5"/>
@@ -16,7 +16,7 @@
     <sheet name="NewUser" r:id="rId7" sheetId="7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:O9"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>パスワード</t>
   </si>
@@ -189,13 +189,43 @@
   <si>
     <t>TestPF1221_05082021123419</t>
   </si>
+  <si>
+    <t>TestPF1221+05082021132632@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_05082021132632</t>
+  </si>
+  <si>
+    <t>TestPF1221+05082021133434@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_05082021133434</t>
+  </si>
+  <si>
+    <t>TestPF1221+05082021133619@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_05082021133619</t>
+  </si>
+  <si>
+    <t>TestPF1221+05082021134218@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_05082021134218</t>
+  </si>
+  <si>
+    <t>TestPF1221+05082021134503@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_05082021134503</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,13 +254,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -246,7 +290,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
@@ -279,6 +323,8 @@
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -594,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -607,7 +653,7 @@
     <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -615,6 +661,7 @@
         <v>1</v>
       </c>
     </row>
+    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.4"/>
   </sheetData>
   <hyperlinks>
     <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A1"/>
@@ -994,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1004,30 +1051,31 @@
     <col min="3" max="3" customWidth="true" width="32.84375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row customFormat="1" r="1" s="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit for order flow
commit for order flow
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sopan\Project\Automation\PlatformTesting\platform\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FE717C58-AB3D-4692-BCB6-FBA2EEAB8696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="20760" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -18,8 +14,10 @@
     <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
     <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
     <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
+    <sheet name="NewUser" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>パスワード</t>
   </si>
@@ -136,9 +134,6 @@
     <t>spoan.patil@scispl.com</t>
   </si>
   <si>
-    <t>sopan181</t>
-  </si>
-  <si>
     <t>2月</t>
   </si>
   <si>
@@ -173,13 +168,71 @@
   </si>
   <si>
     <t>075</t>
+  </si>
+  <si>
+    <t>asas</t>
+  </si>
+  <si>
+    <t>asa</t>
+  </si>
+  <si>
+    <t>asaas</t>
+  </si>
+  <si>
+    <t>氏名（漢字）名は全角文字を入力してください。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+郵便番号形式で入力してください。</t>
+  </si>
+  <si>
+    <t>住所（市区郡）は全角文字を入力してください。</t>
+  </si>
+  <si>
+    <t>氏名（漢字）姓は全角文字を入力してください。</t>
+  </si>
+  <si>
+    <t>氏名（カナ）セイは全角カナ・アルファベットを入力してください。</t>
+  </si>
+  <si>
+    <t>氏名（カナ）メイは全角カナ・アルファベットを入力してください。</t>
+  </si>
+  <si>
+    <t>郵便番号形式で入力してください。</t>
+  </si>
+  <si>
+    <t>住所（丁目・番地）は全角文字を入力してください。</t>
+  </si>
+  <si>
+    <t>住所（町村）は全角文字を入力してください。</t>
+  </si>
+  <si>
+    <t>住所（マンション・ビル名）は全角文字を入力してください。</t>
+  </si>
+  <si>
+    <t>電話番号形式で入力してください。</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Eid</t>
+  </si>
+  <si>
+    <t>rahul80</t>
+  </si>
+  <si>
+    <t>rahul_123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,13 +261,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFE15858"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -263,6 +336,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -577,11 +652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,22 +668,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
+    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -699,7 +774,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -747,7 +822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -767,10 +842,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1">
         <v>2025</v>
@@ -782,7 +857,7 @@
         <v>1213</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -792,7 +867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -901,8 +976,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -910,11 +985,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AK1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,21 +999,36 @@
     <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="11"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="12" max="20" width="9" style="1"/>
+    <col min="21" max="21" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="11"/>
+    <col min="25" max="26" width="9" style="1"/>
+    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="51.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="65.42578125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E1" s="1">
         <v>503</v>
@@ -947,29 +1037,127 @@
         <v>2313</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="L1" s="1">
         <v>9695</v>
       </c>
       <c r="M1" s="1">
         <v>1140</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="1">
+        <v>1</v>
+      </c>
+      <c r="S1" s="1">
+        <v>1</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated code for page visibility
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>パスワード</t>
   </si>
@@ -220,12 +220,24 @@
   <si>
     <t>ExpectedString</t>
   </si>
+  <si>
+    <t>登録されているメールアドレスまたはEiDを入力してください。</t>
+  </si>
+  <si>
+    <t>パスワード再設定のメールをお送りします。</t>
+  </si>
+  <si>
+    <t>ForgotPasswordPageMessage1</t>
+  </si>
+  <si>
+    <t>ForgotPasswordPageMessage2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +280,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF402864"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -290,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -325,6 +343,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -762,13 +781,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="26.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.69140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
@@ -776,6 +799,22 @@
       </c>
       <c r="B1" s="13" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated FooterPage file name.
Updated Footerpage file name to FooterPage_PT90_106 to avoid conflicts in Git.
Added FooterAssert sheet in NewTestData.xlsx.
Handled authentication popup for create account page title assertion.
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sopan\Project\Automation\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahaj Balgunde\git\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDEF51E-F261-48AD-A6DF-C1C09378DA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -18,6 +19,7 @@
     <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
     <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
     <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
+    <sheet name="FooterAssert" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>パスワード</t>
   </si>
@@ -244,11 +246,74 @@
   <si>
     <t>電話番号を入力してください。</t>
   </si>
+  <si>
+    <t>利用規約 - スタギア</t>
+  </si>
+  <si>
+    <t>プライバシーポリシー｜株式会社教育測定研究所（JIEM）</t>
+  </si>
+  <si>
+    <t>特定商取引法 - スタギア</t>
+  </si>
+  <si>
+    <t>スタギアサポートセンター</t>
+  </si>
+  <si>
+    <t>【スタギア 受験の窓口】各種検定・試験をお得に便利に申込み！</t>
+  </si>
+  <si>
+    <t>【スタギア】英検S-CBT｜平日受験がおトク！</t>
+  </si>
+  <si>
+    <t>CASECとは？：Point1 すぐ測定 | CASEC（キャセック） - TOEICスコア・英検級の目安がすぐわかる英語テスト</t>
+  </si>
+  <si>
+    <t>大学入学共通テストの到達度確認！『Z会×スタギア』在宅CBT</t>
+  </si>
+  <si>
+    <t>【スタギア 学習の窓口】英検・漢検・数検の公式学習はスタギア</t>
+  </si>
+  <si>
+    <t>英検公式学習はスタギア | 準1級から5級の合格をサポート</t>
+  </si>
+  <si>
+    <t>漢検公式学習はスタギア | 検定合格から日常学習までサポート</t>
+  </si>
+  <si>
+    <t>【スタギア 情報の窓口】検定・入試・塾などの情報をいち早く</t>
+  </si>
+  <si>
+    <t>スタギア大学受験 | 偏差値や学費などの大学情報満載</t>
+  </si>
+  <si>
+    <t>教育費・教育資金 相談サポート</t>
+  </si>
+  <si>
+    <t>ログイン - スタギア</t>
+  </si>
+  <si>
+    <t>アカウント作成 - スタギア</t>
+  </si>
+  <si>
+    <t>アカウントとセキュリティ - スタギア</t>
+  </si>
+  <si>
+    <t>会員ステータス - スタギア</t>
+  </si>
+  <si>
+    <t>ご利用中のサービス - スタギア</t>
+  </si>
+  <si>
+    <t>ご注文履歴 - スタギア</t>
+  </si>
+  <si>
+    <t>退会確認 - スタギア</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -661,21 +726,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -685,26 +750,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
+    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -783,21 +848,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -806,7 +871,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -815,7 +880,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -831,25 +896,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -876,26 +941,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
@@ -913,7 +978,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -932,7 +997,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -949,7 +1014,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -966,7 +1031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
@@ -985,8 +1050,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -994,46 +1059,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AT1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="11"/>
     <col min="12" max="20" width="9" style="1"/>
-    <col min="21" max="21" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" style="11"/>
     <col min="25" max="26" width="9" style="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="75.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="51.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="51.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="65.42578125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="65.44140625" style="1" customWidth="1"/>
     <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="40.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="40.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="40.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="43.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="40.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="38.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="45.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1177,4 +1242,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC397EFE-1643-4376-B9F4-C7675DEAA21A}">
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New user added in excel
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,28 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\WorkSpace\Project\Workspace\GitPFAutomation\PlatformTesting\platform\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20734" windowHeight="11160" firstSheet="3" activeTab="6"/>
+    <workbookView activeTab="7" firstSheet="4" windowHeight="3343" windowWidth="17760" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q9"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>パスワード</t>
   </si>
@@ -263,11 +260,36 @@
   <si>
     <t>パスワード再設定のメールをお送りします。</t>
   </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>EID</t>
+  </si>
+  <si>
+    <t>TestPF1221+11082021150517@gmail.com</t>
+  </si>
+  <si>
+    <t>pfqa_123</t>
+  </si>
+  <si>
+    <t>TestPF1221_11082021150517</t>
+  </si>
+  <si>
+    <t>TestPF1221+11082021152024@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_11082021152024</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,53 +364,53 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -405,10 +427,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -443,7 +465,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -495,7 +517,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -606,21 +628,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -637,7 +659,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -689,15 +711,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -705,9 +727,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.3828125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.69140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.3828125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.69140625" collapsed="false"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -720,15 +742,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -736,10 +758,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -813,13 +835,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -827,9 +849,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.3828125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.69140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.3828125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.69140625" collapsed="false"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
@@ -861,13 +883,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -875,13 +897,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.3046875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.53515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.84375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.3046875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.53515625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.3828125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.84375" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.15234375" collapsed="false"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
@@ -905,14 +927,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -920,14 +942,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.15234375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.53515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.84375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.15234375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.53515625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.3828125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.84375" collapsed="false"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
@@ -1020,17 +1042,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -1038,34 +1060,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="14.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="11"/>
-    <col min="12" max="20" width="9" style="1"/>
-    <col min="21" max="21" width="14.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" style="11"/>
-    <col min="25" max="26" width="9" style="1"/>
-    <col min="27" max="28" width="52.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="75.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="52.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="51.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="65.3828125" style="1" customWidth="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="40.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="43.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="33.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="40.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="38.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="45.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="33.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9" style="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.84375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.3046875" collapsed="false"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="false"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.84375" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.3046875" collapsed="false"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="false"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="false"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.69140625" collapsed="false"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.3046875" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.69140625" collapsed="false"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.69140625" collapsed="false"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.53515625" collapsed="false"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="false"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.3828125" collapsed="false"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="false"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.84375" collapsed="false"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.3046875" collapsed="false"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.84375" collapsed="false"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.84375" collapsed="false"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.53515625" collapsed="false"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.53515625" collapsed="false"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.84375" collapsed="false"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.35">
@@ -1209,16 +1231,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1249,6 +1271,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row customFormat="1" r="1" s="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new methods to read error string
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="3343" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="3343" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="NewUser" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q9"/>
+  <oleSize ref="A1:O9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1353,7 +1353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>

</xml_diff>

<commit_message>
updated code for writing new password in excel
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sopan\Project\Automation\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\WorkSpace\Project\Workspace\GitPFAutomation\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="5" windowHeight="3375" windowWidth="17760" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="3343" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="User" r:id="rId1" sheetId="5"/>
-    <sheet name="Register" r:id="rId2" sheetId="1"/>
-    <sheet name="Product" r:id="rId3" sheetId="2"/>
-    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
-    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
-    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
-    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
-    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
-    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
+    <sheet name="User" sheetId="5" r:id="rId1"/>
+    <sheet name="Register" sheetId="1" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" r:id="rId3"/>
+    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
+    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
+    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
+    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
+    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
+    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
   <si>
     <t>パスワード</t>
   </si>
@@ -275,15 +275,6 @@
     <t>EID</t>
   </si>
   <si>
-    <t>pfqa_123</t>
-  </si>
-  <si>
-    <t>TestPF1221+11082021152024@gmail.com</t>
-  </si>
-  <si>
-    <t>TestPF1221_11082021152024</t>
-  </si>
-  <si>
     <t>InvalidEmailErrorMessage</t>
   </si>
   <si>
@@ -320,17 +311,19 @@
     <t>プライム会員</t>
   </si>
   <si>
-    <t>TestPF1221+12082021160204@gmail.com</t>
-  </si>
-  <si>
-    <t>TestPF1221_12082021160204</t>
+    <t>TestPF1221+12082021182038@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_12082021182038</t>
+  </si>
+  <si>
+    <t>12082021182154</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,53 +398,53 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -468,10 +461,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -506,7 +499,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -558,7 +551,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -669,21 +662,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -700,7 +693,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -752,28 +745,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="false"/>
-    <col min="3" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="23.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -783,26 +776,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A1"/>
+    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,7 +833,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -876,26 +869,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="false"/>
-    <col min="3" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="23.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -904,7 +897,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -913,7 +906,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -924,30 +917,30 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.5703125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.140625" collapsed="false"/>
-    <col min="7" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="17.3046875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.53515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -968,32 +961,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="1" width="12.140625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="1" width="19.5703125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.85546875" collapsed="false"/>
-    <col min="8" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.53515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
@@ -1011,7 +1004,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1023,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1047,7 +1040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1064,7 +1057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
@@ -1083,55 +1076,55 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
-    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="7" style="1" width="9.0" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="false"/>
-    <col min="11" max="11" style="11" width="9.0" collapsed="false"/>
-    <col min="12" max="20" style="1" width="9.0" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="false"/>
-    <col min="24" max="24" style="11" width="9.0" collapsed="false"/>
-    <col min="25" max="26" style="1" width="9.0" collapsed="false"/>
-    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="false"/>
-    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.28515625" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.7109375" collapsed="false"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="false"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.5703125" collapsed="false"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="false"/>
-    <col min="36" max="36" customWidth="true" style="1" width="65.42578125" collapsed="false"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="false"/>
-    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.85546875" collapsed="false"/>
-    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.28515625" collapsed="false"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.85546875" collapsed="false"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.85546875" collapsed="false"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.5703125" collapsed="false"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="false"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.85546875" collapsed="false"/>
-    <col min="47" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="7" width="9" style="1" collapsed="1"/>
+    <col min="8" max="8" width="14.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9" style="11" collapsed="1"/>
+    <col min="12" max="20" width="9" style="1" collapsed="1"/>
+    <col min="21" max="21" width="14.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="11" collapsed="1"/>
+    <col min="25" max="26" width="9" style="1" collapsed="1"/>
+    <col min="27" max="28" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1272,25 +1265,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="false"/>
+    <col min="1" max="1" width="26.3046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>67</v>
       </c>
@@ -1298,7 +1291,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1306,7 +1299,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1314,70 +1307,70 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
         <v>79</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>81</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>83</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>85</v>
       </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row customFormat="1" r="1" s="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -1388,47 +1381,47 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="false"/>
-    <col min="2" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="10.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working code for invalid reset password
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\WorkSpace\Project\Workspace\GitPFAutomation\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="3343" firstSheet="5" activeTab="7"/>
+    <workbookView activeTab="7" firstSheet="5" windowHeight="3343" windowWidth="17760" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
-    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
-    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
+    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
   <si>
     <t>パスワード</t>
   </si>
@@ -319,11 +319,21 @@
   <si>
     <t>12082021182154</t>
   </si>
+  <si>
+    <t>TestPF1221+13082021092544@gmail.com</t>
+  </si>
+  <si>
+    <t>pfqa_123</t>
+  </si>
+  <si>
+    <t>TestPF1221_13082021092544</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,53 +408,53 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -461,10 +471,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -499,7 +509,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -551,7 +561,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -662,21 +672,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -693,7 +703,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -745,15 +755,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -761,9 +771,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.3828125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.3828125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.69140625" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -776,15 +786,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -792,10 +802,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +843,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -869,13 +879,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -883,9 +893,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.3828125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.3828125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.69140625" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
@@ -917,13 +927,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -931,13 +941,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.3046875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.53515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.3046875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.53515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.3828125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.84375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.15234375" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
@@ -961,14 +971,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -976,14 +986,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.53515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.15234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.53515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.3828125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.84375" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
@@ -1076,17 +1086,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -1094,34 +1104,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9" style="11" collapsed="1"/>
-    <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="11" collapsed="1"/>
-    <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.3828125" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.84375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.3046875" collapsed="true"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.84375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.3046875" collapsed="true"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.69140625" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.3046875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.69140625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.69140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.53515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.3828125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.84375" collapsed="true"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.3046875" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.84375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.84375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.53515625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.53515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.84375" collapsed="true"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.35">
@@ -1265,14 +1275,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
@@ -1280,7 +1290,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.3046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.3046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -1356,13 +1366,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1370,7 +1380,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.4">
+    <row customFormat="1" r="1" s="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -1381,26 +1391,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -1408,8 +1418,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.15234375" collapsed="true"/>
+    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -1421,7 +1431,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complete all test script
complete all test script
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FE717C58-AB3D-4692-BCB6-FBA2EEAB8696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85653F1C-241A-40BB-BC56-B33076CACC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="20760" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -17,7 +22,6 @@
     <sheet name="NewUser" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>パスワード</t>
   </si>
@@ -227,12 +231,15 @@
   <si>
     <t>rahul_123</t>
   </si>
+  <si>
+    <t>UserName</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +278,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -653,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,16 +680,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -687,12 +709,13 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -988,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK1"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AJ9" sqref="AJ9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update NewTestData.xlsx for Footer and Terms Conditions Assert
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahaj Balgunde\git\PlatformTesting\platform\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F7811B-60A8-4BC3-826B-0BC51A02361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17760" windowHeight="11020" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="3996" yWindow="3540" windowWidth="17280" windowHeight="9420" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -18,6 +24,8 @@
     <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
     <sheet name="Header" sheetId="10" r:id="rId10"/>
     <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
+    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="132">
   <si>
     <t>パスワード</t>
   </si>
@@ -337,11 +345,113 @@
   <si>
     <t>ご注文内容</t>
   </si>
+  <si>
+    <t>利用規約 - スタギア</t>
+  </si>
+  <si>
+    <t>プライバシーポリシー｜株式会社教育測定研究所（JIEM）</t>
+  </si>
+  <si>
+    <t>特定商取引法 - スタギア</t>
+  </si>
+  <si>
+    <t>スタギアサポートセンター</t>
+  </si>
+  <si>
+    <t>【スタギア】英検S-CBT｜平日受験がおトク！</t>
+  </si>
+  <si>
+    <t>CASECとは？：Point1 すぐ測定 | CASEC（キャセック） - TOEICスコア・英検級の目安がすぐわかる英語テスト</t>
+  </si>
+  <si>
+    <t>大学入学共通テストの到達度確認！『Z会×スタギア』在宅CBT</t>
+  </si>
+  <si>
+    <t>英検公式学習はスタギア | 準1級から5級の合格をサポート</t>
+  </si>
+  <si>
+    <t>漢検公式学習はスタギア | 検定合格から日常学習までサポート</t>
+  </si>
+  <si>
+    <t>スタギア大学受験 | 偏差値や学費などの大学情報満載</t>
+  </si>
+  <si>
+    <t>教育費・教育資金 相談サポート</t>
+  </si>
+  <si>
+    <t>アカウント作成 - スタギア</t>
+  </si>
+  <si>
+    <t>アカウントとセキュリティ - スタギア</t>
+  </si>
+  <si>
+    <t>会員ステータス - スタギア</t>
+  </si>
+  <si>
+    <t>ご利用中のサービス - スタギア</t>
+  </si>
+  <si>
+    <t>ご注文履歴 - スタギア</t>
+  </si>
+  <si>
+    <t>退会確認 - スタギア</t>
+  </si>
+  <si>
+    <t>CASEC/英語コミュニケーション能力判定テスト・キャセック</t>
+  </si>
+  <si>
+    <t>利用規約 | 塾ピタ - 学習塾・予備校の検索・体験予約なら</t>
+  </si>
+  <si>
+    <t>利用規約【スタギア大学受験】</t>
+  </si>
+  <si>
+    <t>ユーザー利用規約 | 教育費・教育資金 相談サポート</t>
+  </si>
+  <si>
+    <t>利用規約・個人情報の取扱 | 英ナビ！</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Privacy Policy</t>
+  </si>
+  <si>
+    <t>カスタマイズされた広告のプライバシーに関するユーザーのオプション | Twitterヘルプ</t>
+  </si>
+  <si>
+    <t>LINEプライバシーポリシー</t>
+  </si>
+  <si>
+    <t>当社によるウェブサイト訪問履歴情報とLINEアカウントとの関連付けの停止(オプトアウト)について</t>
+  </si>
+  <si>
+    <t>Amazon.co.jp ヘルプ: パーソナライズド広告規約</t>
+  </si>
+  <si>
+    <t>Amazon.co.jp: Advertising Preferences</t>
+  </si>
+  <si>
+    <t>個人情報のお取り扱いについて｜株式会社ブレインパッド</t>
+  </si>
+  <si>
+    <t>個人情報保護方針｜OPEN DX - 株式会社EVERRISE</t>
+  </si>
+  <si>
+    <t>NAI Consumer Opt Out</t>
+  </si>
+  <si>
+    <t>WebChoices: Digital Advertising Alliance's Consumer Choice Tool for Web US</t>
+  </si>
+  <si>
+    <t>オプトアウト等 – DDAI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -459,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -507,6 +617,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -814,28 +927,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -845,23 +958,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
+    <hyperlink ref="A1" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5">
+    <row r="1" spans="1:9" ht="17.399999999999999">
       <c r="A1" s="16" t="s">
         <v>91</v>
       </c>
@@ -889,19 +1002,254 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
+        <v>112</v>
+      </c>
+      <c r="U1" t="s">
+        <v>113</v>
+      </c>
+      <c r="V1" t="s">
+        <v>114</v>
+      </c>
+      <c r="W1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="56.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.44140625" customWidth="1"/>
+    <col min="15" max="15" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="64.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" t="s">
+        <v>129</v>
+      </c>
+      <c r="S1" t="s">
+        <v>130</v>
+      </c>
+      <c r="T1" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -910,19 +1258,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29">
+    <row r="1" spans="1:12" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +1308,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29">
+    <row r="2" spans="1:12" ht="28.8">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1001,21 +1349,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1049,21 +1397,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.453125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.81640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.21875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1094,22 +1442,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.1796875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.453125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.21875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.77734375" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1203,8 +1551,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1212,42 +1560,42 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="9" style="11" collapsed="1"/>
     <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" style="11" collapsed="1"/>
     <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.6328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="28" width="52.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.6328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.6328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.33203125" style="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1398,19 +1746,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2">
       <c r="A1" s="14" t="s">
         <v>67</v>
       </c>
@@ -1488,14 +1836,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
@@ -1526,16 +1874,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.21875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
commit for prime flow and , update method name
commit for prime flow and , update method name
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF2A748-DBB4-4059-BDDD-D473FEF66E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF5CED1-7C66-4140-9314-FA28385189E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
     <sheet name="NewUser" sheetId="8" r:id="rId8"/>
     <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
+    <sheet name="CommonForOrder" sheetId="10" r:id="rId10"/>
+    <sheet name="Step 2 validation" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>パスワード</t>
   </si>
@@ -322,6 +324,9 @@
   </si>
   <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>TaxForProducts</t>
   </si>
 </sst>
 </file>
@@ -759,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -794,12 +799,55 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5E4C2A-2822-4145-AC61-CEA202F8B9D3}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FBABDF-AD61-4F00-9193-49792663E7BE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
NewTestData update for Withdrawal Account
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahaj Balgunde\git\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4024FA63-EB01-4ED3-8EA7-CC656279C473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21163971-A5E8-4EC5-B941-3B98F68AC448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
     <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
     <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
+    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="134">
   <si>
     <t>パスワード</t>
   </si>
@@ -449,6 +450,9 @@
   </si>
   <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>sahaj_automate</t>
   </si>
 </sst>
 </file>
@@ -940,14 +944,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" activeCellId="1" sqref="A1:XFD2 B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -983,9 +987,9 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:9" ht="17.399999999999999">
       <c r="A1" s="16" t="s">
         <v>91</v>
       </c>
@@ -1018,9 +1022,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1041,37 +1045,37 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1179,29 +1183,29 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.44140625" customWidth="1"/>
+    <col min="15" max="15" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="64.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row r="1" spans="1:20" ht="28.8">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -1261,6 +1265,32 @@
       </c>
       <c r="T1" t="s">
         <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1276,12 +1306,12 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row r="1" spans="1:12" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1349,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="28.8">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1367,10 +1397,10 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1415,14 +1445,14 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1460,15 +1490,15 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1578,35 +1608,35 @@
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="9" style="11" collapsed="1"/>
     <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" style="11" collapsed="1"/>
     <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="28" width="52.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.33203125" style="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1764,9 +1794,9 @@
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1854,7 +1884,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
@@ -1892,9 +1922,9 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update NewTestData with Withdrawal Account
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahaj Balgunde\git\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21163971-A5E8-4EC5-B941-3B98F68AC448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88472003-3D88-4577-B96C-5CA372DC1693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="134">
   <si>
     <t>パスワード</t>
   </si>
@@ -945,7 +945,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" activeCellId="1" sqref="A1:XFD2 B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1274,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1286,10 +1286,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>133</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extent Report with Complete Suite Execution
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahaj Balgunde\git\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88472003-3D88-4577-B96C-5CA372DC1693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{88472003-3D88-4577-B96C-5CA372DC1693}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="13" firstSheet="10" windowHeight="9420" windowWidth="17280" xWindow="384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="384"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
-    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
-    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
-    <sheet name="Header" sheetId="10" r:id="rId10"/>
-    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
-    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
-    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
-    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId14"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
+    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
+    <sheet name="Header" r:id="rId10" sheetId="10"/>
+    <sheet name="MemberPlanAssert" r:id="rId11" sheetId="11"/>
+    <sheet name="FooterAssert" r:id="rId12" sheetId="12"/>
+    <sheet name="FooterTermsAssert" r:id="rId13" sheetId="13"/>
+    <sheet name="WithdrawalAccount" r:id="rId14" sheetId="14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="136">
   <si>
     <t>パスワード</t>
   </si>
@@ -454,11 +454,18 @@
   <si>
     <t>sahaj_automate</t>
   </si>
+  <si>
+    <t>TestPF1221+17082021184752@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_17082021184752</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -573,67 +580,67 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -650,10 +657,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -688,7 +695,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -740,7 +747,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -851,21 +858,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -882,7 +889,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -934,15 +941,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -950,9 +957,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.6640625" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -973,15 +980,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -989,7 +996,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999">
+    <row ht="17.399999999999999" r="1" spans="1:9">
       <c r="A1" s="16" t="s">
         <v>91</v>
       </c>
@@ -1012,19 +1019,19 @@
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.33203125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1033,13 +1040,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
-  <dimension ref="A1:AD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -1047,35 +1054,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.88671875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.6640625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="42.6640625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="99.88671875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="57.33203125" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="60.6640625" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="53.88671875" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="58.6640625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="60.6640625" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="49.6640625" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.88671875" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="35.33203125" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="24.88671875" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.6640625" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="22.88671875" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1171,13 +1178,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1185,27 +1192,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.44140625" customWidth="1"/>
-    <col min="15" max="15" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.33203125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="53.44140625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.33203125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.44140625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.109375" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="92.109375" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="41.44140625" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="32.6640625" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="54.33203125" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5546875" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.6640625" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5546875" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="21.33203125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8">
+    <row ht="28.8" r="1" spans="1:20">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -1268,13 +1275,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1282,7 +1289,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="14.33203125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1302,13 +1309,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -1316,10 +1323,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8">
+    <row ht="28.8" r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8">
+    <row ht="28.8" r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1393,13 +1400,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1407,9 +1414,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.6640625" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1441,13 +1448,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1455,13 +1462,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.33203125" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1485,14 +1492,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1500,14 +1507,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.6640625" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1600,17 +1607,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -1618,34 +1625,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9" style="11" collapsed="1"/>
-    <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="11" collapsed="1"/>
-    <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.33203125" collapsed="true"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.33203125" collapsed="true"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.6640625" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.33203125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.6640625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.6640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.44140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.33203125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.6640625" collapsed="true"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.33203125" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.6640625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.6640625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.44140625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.44140625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.6640625" collapsed="true"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -1789,14 +1796,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
@@ -1804,7 +1811,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1880,13 +1887,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1894,7 +1901,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1">
+    <row customFormat="1" r="1" s="14" spans="1:3">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -1905,26 +1912,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -1932,8 +1939,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.33203125" collapsed="true"/>
+    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1945,7 +1952,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit payment credit card
commit payment credit card
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,35 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4024FA63-EB01-4ED3-8EA7-CC656279C473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6FAD3A21-CE18-4C6B-A6DD-CF65703EDE35}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="13" firstSheet="9" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
-    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
-    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
-    <sheet name="Header" sheetId="10" r:id="rId10"/>
-    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
-    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
-    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
+    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
+    <sheet name="Header" r:id="rId10" sheetId="10"/>
+    <sheet name="MemberPlanAssert" r:id="rId11" sheetId="11"/>
+    <sheet name="FooterAssert" r:id="rId12" sheetId="12"/>
+    <sheet name="FooterTermsAssert" r:id="rId13" sheetId="13"/>
+    <sheet name="CreditCardTestData" r:id="rId14" sheetId="14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
   <si>
     <t>パスワード</t>
   </si>
@@ -316,15 +317,9 @@
     <t>プライム会員</t>
   </si>
   <si>
-    <t>TestPF1221+13082021092544@gmail.com</t>
-  </si>
-  <si>
     <t>pfqa_123</t>
   </si>
   <si>
-    <t>TestPF1221_13082021092544</t>
-  </si>
-  <si>
     <t>【スタギア 受験の窓口】各種検定・試験をお得に便利に申込み！</t>
   </si>
   <si>
@@ -449,12 +444,49 @@
   </si>
   <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>ValidCreditCardNumer</t>
+  </si>
+  <si>
+    <t>ExpirationYear</t>
+  </si>
+  <si>
+    <t>CreditCardHolderName</t>
+  </si>
+  <si>
+    <t>SecurityCode</t>
+  </si>
+  <si>
+    <t>ExpirationMonth</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>7月</t>
+  </si>
+  <si>
+    <t>InValidCreditCardNumer</t>
+  </si>
+  <si>
+    <t>TestPF1221+17082021184550@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_17082021184550</t>
+  </si>
+  <si>
+    <t>TestPF1221+17082021185316@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_17082021185316</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -569,67 +601,67 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -646,10 +678,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -684,7 +716,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -736,7 +768,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -847,21 +879,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -878,7 +910,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -930,30 +962,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" activeCellId="1" sqref="A1:XFD2 B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="7" style="1" width="9.0" collapsed="false"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>74</v>
@@ -969,15 +1002,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -985,57 +1018,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row ht="18" r="1" spans="1:9">
       <c r="A1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="G1" s="19"/>
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
-  <dimension ref="A1:AD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -1043,137 +1076,137 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="42.7109375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="99.85546875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="57.28515625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="53.85546875" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="58.7109375" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="49.7109375" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.85546875" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="35.28515625" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="24.85546875" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.7109375" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" t="s">
         <v>107</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" t="s">
+        <v>99</v>
+      </c>
+      <c r="X1" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" t="s">
-        <v>112</v>
-      </c>
-      <c r="U1" t="s">
-        <v>113</v>
-      </c>
-      <c r="V1" t="s">
-        <v>114</v>
-      </c>
-      <c r="W1" t="s">
-        <v>101</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>101</v>
-      </c>
       <c r="AB1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD1" t="s">
         <v>98</v>
       </c>
-      <c r="AC1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1181,96 +1214,165 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="53.42578125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5703125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.28515625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5703125" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.140625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="92.140625" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="41.42578125" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="32.7109375" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="54.28515625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5703125" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5703125" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row ht="30" r="1" spans="1:20">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>116</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>117</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
         <v>118</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
         <v>119</v>
       </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>120</v>
       </c>
-      <c r="I1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>121</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>122</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>124</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="P1" t="s">
         <v>125</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>126</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>128</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>129</v>
       </c>
-      <c r="S1" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" t="s">
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB7314A-3160-4A43-AA7B-8735E410A44B}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="21.5703125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="22.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="45.85546875" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="9" t="s">
         <v>131</v>
       </c>
+      <c r="B1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2025</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -1278,10 +1380,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row ht="30" r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1421,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row ht="30" r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1355,13 +1457,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1369,9 +1471,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1403,13 +1505,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1417,13 +1519,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1447,14 +1549,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1462,14 +1564,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1562,17 +1664,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -1580,34 +1682,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9" style="11" collapsed="1"/>
-    <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="11" collapsed="1"/>
-    <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.7109375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -1751,14 +1853,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
@@ -1766,7 +1868,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1842,21 +1944,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.42578125" collapsed="false"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1">
+    <row customFormat="1" r="1" s="14" spans="1:3">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -1867,26 +1974,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -1894,8 +2001,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1907,7 +2014,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove string hard code
remove string hard code
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,36 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6FAD3A21-CE18-4C6B-A6DD-CF65703EDE35}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2E7EBA-1649-49BE-A0E2-971877F9BCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="9" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User" r:id="rId1" sheetId="5"/>
-    <sheet name="Register" r:id="rId2" sheetId="1"/>
-    <sheet name="Product" r:id="rId3" sheetId="2"/>
-    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
-    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
-    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
-    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
-    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
-    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
-    <sheet name="Header" r:id="rId10" sheetId="10"/>
-    <sheet name="MemberPlanAssert" r:id="rId11" sheetId="11"/>
-    <sheet name="FooterAssert" r:id="rId12" sheetId="12"/>
-    <sheet name="FooterTermsAssert" r:id="rId13" sheetId="13"/>
-    <sheet name="CreditCardTestData" r:id="rId14" sheetId="14"/>
+    <sheet name="User" sheetId="5" r:id="rId1"/>
+    <sheet name="Register" sheetId="1" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" r:id="rId3"/>
+    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
+    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
+    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
+    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
+    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
+    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
+    <sheet name="Header" sheetId="10" r:id="rId10"/>
+    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
+    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
+    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
+    <sheet name="CreditCardTestData" sheetId="14" r:id="rId14"/>
+    <sheet name="Order" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="184">
   <si>
     <t>パスワード</t>
   </si>
@@ -470,23 +471,145 @@
     <t>InValidCreditCardNumer</t>
   </si>
   <si>
-    <t>TestPF1221+17082021184550@gmail.com</t>
-  </si>
-  <si>
-    <t>TestPF1221_17082021184550</t>
-  </si>
-  <si>
-    <t>TestPF1221+17082021185316@gmail.com</t>
-  </si>
-  <si>
-    <t>TestPF1221_17082021185316</t>
+    <t>expectedInvalidCreditCardText</t>
+  </si>
+  <si>
+    <t>ご利用いただけないクレジットカードです。</t>
+  </si>
+  <si>
+    <t>expectedBlankCreditCardText</t>
+  </si>
+  <si>
+    <t>入力してください</t>
+  </si>
+  <si>
+    <t>柏木佳　奈子</t>
+  </si>
+  <si>
+    <t>カシワギ　カナコ</t>
+  </si>
+  <si>
+    <t>rahul.shinde+82@scispl.com</t>
+  </si>
+  <si>
+    <t>rahul.shinde</t>
+  </si>
+  <si>
+    <t>validConStoreKanjiName</t>
+  </si>
+  <si>
+    <t>validConStoreKanaName</t>
+  </si>
+  <si>
+    <t>validConStorePhoneno</t>
+  </si>
+  <si>
+    <t>validConStoreEmailAddress</t>
+  </si>
+  <si>
+    <t>InValidConStoreEmailAddress</t>
+  </si>
+  <si>
+    <t>expectedinvalidEmailConStoreText</t>
+  </si>
+  <si>
+    <t>有効なメールアドレスを入力してください</t>
+  </si>
+  <si>
+    <t>expectedBlankConStoreText</t>
+  </si>
+  <si>
+    <t>氏名（漢字）を入力してください</t>
+  </si>
+  <si>
+    <t>expectedKanaConStoreText</t>
+  </si>
+  <si>
+    <t>氏名（カナ）を入力してください</t>
+  </si>
+  <si>
+    <t>expectedTelePhoneConStoreText</t>
+  </si>
+  <si>
+    <t>電話番号を入力してください</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageExpectedBuyAgainButton</t>
+  </si>
+  <si>
+    <t>再度購入</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageExpectedStatusPaymentUnconfirmed</t>
+  </si>
+  <si>
+    <t>支払い未確認</t>
+  </si>
+  <si>
+    <t>ご購入ありがとうございます。</t>
+  </si>
+  <si>
+    <t>ThankYouPageThankYouForYourApplicationLabel</t>
+  </si>
+  <si>
+    <t>今すぐはじめる</t>
+  </si>
+  <si>
+    <t>startNowButtonSTRStartNowButton</t>
+  </si>
+  <si>
+    <t>ありがとうございます！</t>
+  </si>
+  <si>
+    <t>ThankYouPageThankYouForPrimeLabel</t>
+  </si>
+  <si>
+    <t>ThankYouPageTopPageButton</t>
+  </si>
+  <si>
+    <t>トップページ</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageStatusPaymentconfirmed</t>
+  </si>
+  <si>
+    <t>支払い確認済み</t>
+  </si>
+  <si>
+    <t>PrimeLabel</t>
+  </si>
+  <si>
+    <t>プライム会員プラン</t>
+  </si>
+  <si>
+    <t>PrimePrice</t>
+  </si>
+  <si>
+    <t>PrimeButtonOnHeaderPage</t>
+  </si>
+  <si>
+    <t>クレジットカード支払い</t>
+  </si>
+  <si>
+    <t>MembershipPagePrimeCreditCardLabel</t>
+  </si>
+  <si>
+    <t>LearnButtonLabelForKankenProduct</t>
+  </si>
+  <si>
+    <t>TestPF1221+18082021183337@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_18082021183337</t>
+  </si>
+  <si>
+    <t>近日公開</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -601,67 +724,68 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -678,10 +802,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -716,7 +840,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -768,7 +892,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -879,21 +1003,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -910,7 +1034,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -962,15 +1086,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:K1048576"/>
@@ -978,10 +1102,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
-    <col min="3" max="7" style="1" width="9.0" collapsed="false"/>
-    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1002,15 +1125,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -1018,7 +1141,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row ht="18" r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1041,19 +1164,19 @@
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.28515625" collapsed="false"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1062,13 +1185,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
-  <dimension ref="A1:AE1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -1076,35 +1199,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="42.7109375" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="99.85546875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="57.28515625" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="53.85546875" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="58.7109375" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="49.7109375" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="24.85546875" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="35.28515625" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="24.85546875" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="20.7109375" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1200,13 +1323,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
-  <dimension ref="A1:U1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1214,27 +1337,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.28515625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="53.42578125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5703125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="48.28515625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5703125" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="25.140625" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="92.140625" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="41.42578125" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="32.7109375" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="54.28515625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5703125" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5703125" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
+    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="41.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:20">
+    <row r="1" spans="1:20" ht="30">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1297,28 +1420,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB7314A-3160-4A43-AA7B-8735E410A44B}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB7314A-3160-4A43-AA7B-8735E410A44B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="9" width="21.5703125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="22.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="45.85546875" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="21.5703125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="45.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1365,14 +1488,205 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A9CD38-1ED9-4BA0-9A34-A15D2614D5D9}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="36.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="51.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="41.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="34.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="48.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="45.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O1" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S1" t="s">
+        <v>172</v>
+      </c>
+      <c r="T1" t="s">
+        <v>174</v>
+      </c>
+      <c r="U1" t="s">
+        <v>176</v>
+      </c>
+      <c r="V1" t="s">
+        <v>177</v>
+      </c>
+      <c r="W1" t="s">
+        <v>179</v>
+      </c>
+      <c r="X1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2">
+        <v>9890324119</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L2" t="s">
+        <v>159</v>
+      </c>
+      <c r="M2" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>168</v>
+      </c>
+      <c r="R2" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T2" t="s">
+        <v>175</v>
+      </c>
+      <c r="U2">
+        <v>500</v>
+      </c>
+      <c r="V2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>178</v>
+      </c>
+      <c r="X2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{6C31F2E5-ACAB-49C8-B2BB-F2F9F15554C8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -1380,10 +1694,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1421,7 +1735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1457,13 +1771,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1471,9 +1785,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1505,13 +1819,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1519,13 +1833,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.28515625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1549,14 +1863,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1564,14 +1878,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1664,17 +1978,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AU1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -1682,34 +1996,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
-    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
-    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
-    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
-    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
-    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
-    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.7109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.42578125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="65.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
-    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
-    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.42578125" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
-    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="7" width="9" style="1" collapsed="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9" style="11" collapsed="1"/>
+    <col min="12" max="20" width="9" style="1" collapsed="1"/>
+    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="11" collapsed="1"/>
+    <col min="25" max="26" width="9" style="1" collapsed="1"/>
+    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -1853,22 +2167,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1944,13 +2258,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
@@ -1958,12 +2272,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.42578125" collapsed="false"/>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="14" spans="1:3">
+    <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -1974,26 +2288,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -2001,8 +2315,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
-    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2014,7 +2328,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add data in excel for prime user
add data in excel for prime user
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2E7EBA-1649-49BE-A0E2-971877F9BCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{AB56E10B-7161-4FE5-8203-4A8DD9DA942A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="15" firstSheet="11" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
-    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
-    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
-    <sheet name="Header" sheetId="10" r:id="rId10"/>
-    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
-    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
-    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
-    <sheet name="CreditCardTestData" sheetId="14" r:id="rId14"/>
-    <sheet name="Order" sheetId="15" r:id="rId15"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
+    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
+    <sheet name="Header" r:id="rId10" sheetId="10"/>
+    <sheet name="MemberPlanAssert" r:id="rId11" sheetId="11"/>
+    <sheet name="FooterAssert" r:id="rId12" sheetId="12"/>
+    <sheet name="FooterTermsAssert" r:id="rId13" sheetId="13"/>
+    <sheet name="CreditCardTestData" r:id="rId14" sheetId="14"/>
+    <sheet name="Order" r:id="rId15" sheetId="15"/>
+    <sheet name="PrimeUser" r:id="rId16" sheetId="16"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="190">
   <si>
     <t>パスワード</t>
   </si>
@@ -605,11 +606,30 @@
   <si>
     <t>近日公開</t>
   </si>
+  <si>
+    <t>TestPF1221+19082021104803@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_19082021104803</t>
+  </si>
+  <si>
+    <t>TestPF1221+19082021105502@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_19082021105502</t>
+  </si>
+  <si>
+    <t>TestPF1221+19082021110338@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_19082021110338</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -724,68 +744,68 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -802,10 +822,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -840,7 +860,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -892,7 +912,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1003,21 +1023,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1034,7 +1054,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1086,15 +1106,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:K1048576"/>
@@ -1102,9 +1122,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1125,15 +1145,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -1141,7 +1161,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row ht="18" r="1" spans="1:9">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1164,19 +1184,19 @@
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1185,13 +1205,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
-  <dimension ref="A1:AD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -1199,35 +1219,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="54" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="54" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="99.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="57.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="53.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="58.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="49.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1323,13 +1343,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1337,27 +1357,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="54" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="53.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="92.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row ht="30" r="1" spans="1:20">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1420,13 +1440,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB7314A-3160-4A43-AA7B-8735E410A44B}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB7314A-3160-4A43-AA7B-8735E410A44B}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -1434,14 +1454,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="45.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="16.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="22.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="45.85546875" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1488,44 +1508,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A9CD38-1ED9-4BA0-9A34-A15D2614D5D9}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A9CD38-1ED9-4BA0-9A34-A15D2614D5D9}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="36.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="51.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="41.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="48.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="45.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="48.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="10" max="11" bestFit="true" customWidth="true" width="36.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="31.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="51.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="45.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1678,15 +1698,41 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{6C31F2E5-ACAB-49C8-B2BB-F2F9F15554C8}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{6C31F2E5-ACAB-49C8-B2BB-F2F9F15554C8}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE733D7C-6839-4F21-B77B-279D31AADD2A}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -1694,10 +1740,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row ht="30" r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row ht="30" r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1771,13 +1817,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1785,9 +1831,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1819,13 +1865,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1833,13 +1879,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1863,14 +1909,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1878,14 +1924,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1978,17 +2024,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -1996,34 +2042,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9" style="11" collapsed="1"/>
-    <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="11" collapsed="1"/>
-    <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.7109375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -2167,14 +2213,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2182,7 +2228,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2258,26 +2304,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1">
+    <row customFormat="1" r="1" s="14" spans="1:3">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -2288,26 +2334,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -2315,8 +2361,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2328,7 +2374,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push rahul excel file
push rahul excel file
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahaj Balgunde\git\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{88472003-3D88-4577-B96C-5CA372DC1693}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023E4A77-41E6-40E8-8684-B1FF821B9451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="10" windowHeight="9420" windowWidth="17280" xWindow="384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="384"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User" r:id="rId1" sheetId="5"/>
-    <sheet name="Register" r:id="rId2" sheetId="1"/>
-    <sheet name="Product" r:id="rId3" sheetId="2"/>
-    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
-    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
-    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
-    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
-    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
-    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
-    <sheet name="Header" r:id="rId10" sheetId="10"/>
-    <sheet name="MemberPlanAssert" r:id="rId11" sheetId="11"/>
-    <sheet name="FooterAssert" r:id="rId12" sheetId="12"/>
-    <sheet name="FooterTermsAssert" r:id="rId13" sheetId="13"/>
-    <sheet name="WithdrawalAccount" r:id="rId14" sheetId="14"/>
+    <sheet name="User" sheetId="5" r:id="rId1"/>
+    <sheet name="Register" sheetId="1" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" r:id="rId3"/>
+    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
+    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
+    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
+    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
+    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
+    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
+    <sheet name="Header" sheetId="10" r:id="rId10"/>
+    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
+    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
+    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
+    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId14"/>
+    <sheet name="Order" sheetId="15" r:id="rId15"/>
+    <sheet name="PrimeUser" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="179">
   <si>
     <t>パスワード</t>
   </si>
@@ -317,15 +319,9 @@
     <t>プライム会員</t>
   </si>
   <si>
-    <t>TestPF1221+13082021092544@gmail.com</t>
-  </si>
-  <si>
     <t>pfqa_123</t>
   </si>
   <si>
-    <t>TestPF1221_13082021092544</t>
-  </si>
-  <si>
     <t>【スタギア 受験の窓口】各種検定・試験をお得に便利に申込み！</t>
   </si>
   <si>
@@ -459,13 +455,147 @@
   </si>
   <si>
     <t>TestPF1221_17082021184752</t>
+  </si>
+  <si>
+    <t>expectedInvalidCreditCardText</t>
+  </si>
+  <si>
+    <t>expectedBlankCreditCardText</t>
+  </si>
+  <si>
+    <t>validConStoreKanjiName</t>
+  </si>
+  <si>
+    <t>validConStoreKanaName</t>
+  </si>
+  <si>
+    <t>validConStorePhoneno</t>
+  </si>
+  <si>
+    <t>validConStoreEmailAddress</t>
+  </si>
+  <si>
+    <t>InValidConStoreEmailAddress</t>
+  </si>
+  <si>
+    <t>expectedinvalidEmailConStoreText</t>
+  </si>
+  <si>
+    <t>expectedBlankConStoreText</t>
+  </si>
+  <si>
+    <t>expectedKanaConStoreText</t>
+  </si>
+  <si>
+    <t>expectedTelePhoneConStoreText</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageExpectedBuyAgainButton</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageExpectedStatusPaymentUnconfirmed</t>
+  </si>
+  <si>
+    <t>ThankYouPageThankYouForYourApplicationLabel</t>
+  </si>
+  <si>
+    <t>startNowButtonSTRStartNowButton</t>
+  </si>
+  <si>
+    <t>ThankYouPageThankYouForPrimeLabel</t>
+  </si>
+  <si>
+    <t>ThankYouPageTopPageButton</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageStatusPaymentconfirmed</t>
+  </si>
+  <si>
+    <t>PrimeLabel</t>
+  </si>
+  <si>
+    <t>PrimePrice</t>
+  </si>
+  <si>
+    <t>PrimeButtonOnHeaderPage</t>
+  </si>
+  <si>
+    <t>MembershipPagePrimeCreditCardLabel</t>
+  </si>
+  <si>
+    <t>LearnButtonLabelForKankenProduct</t>
+  </si>
+  <si>
+    <t>ご利用いただけないクレジットカードです。</t>
+  </si>
+  <si>
+    <t>入力してください</t>
+  </si>
+  <si>
+    <t>柏木佳　奈子</t>
+  </si>
+  <si>
+    <t>カシワギ　カナコ</t>
+  </si>
+  <si>
+    <t>rahul.shinde+82@scispl.com</t>
+  </si>
+  <si>
+    <t>rahul.shinde</t>
+  </si>
+  <si>
+    <t>有効なメールアドレスを入力してください</t>
+  </si>
+  <si>
+    <t>氏名（漢字）を入力してください</t>
+  </si>
+  <si>
+    <t>氏名（カナ）を入力してください</t>
+  </si>
+  <si>
+    <t>電話番号を入力してください</t>
+  </si>
+  <si>
+    <t>再度購入</t>
+  </si>
+  <si>
+    <t>支払い未確認</t>
+  </si>
+  <si>
+    <t>ご購入ありがとうございます。</t>
+  </si>
+  <si>
+    <t>今すぐはじめる</t>
+  </si>
+  <si>
+    <t>ありがとうございます！</t>
+  </si>
+  <si>
+    <t>トップページ</t>
+  </si>
+  <si>
+    <t>支払い確認済み</t>
+  </si>
+  <si>
+    <t>プライム会員プラン</t>
+  </si>
+  <si>
+    <t>クレジットカード支払い</t>
+  </si>
+  <si>
+    <t>近日公開</t>
+  </si>
+  <si>
+    <t>TestPF1221+19082021181704@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_19082021181704</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -580,67 +710,68 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -657,10 +788,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -695,7 +826,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -747,7 +878,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -858,21 +989,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -889,7 +1020,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -941,30 +1072,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.6640625" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>74</v>
@@ -980,321 +1111,321 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row ht="17.399999999999999" r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="G1" s="19"/>
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
-  <dimension ref="A1:AE1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.88671875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="60.6640625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="42.6640625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="99.88671875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="57.33203125" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="60.6640625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="53.88671875" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="58.6640625" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="60.6640625" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="49.6640625" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="24.88671875" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="35.33203125" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="24.88671875" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="20.6640625" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="22.88671875" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="18.6640625" collapsed="false"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.88671875" collapsed="false"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" t="s">
         <v>107</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" t="s">
+        <v>99</v>
+      </c>
+      <c r="X1" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" t="s">
-        <v>112</v>
-      </c>
-      <c r="U1" t="s">
-        <v>113</v>
-      </c>
-      <c r="V1" t="s">
-        <v>114</v>
-      </c>
-      <c r="W1" t="s">
-        <v>101</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>101</v>
-      </c>
       <c r="AB1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD1" t="s">
         <v>98</v>
       </c>
-      <c r="AC1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
-  <dimension ref="A1:U1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.33203125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="53.44140625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5546875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="48.33203125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="35.44140625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.44140625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5546875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="25.109375" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="92.109375" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="41.44140625" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="32.6640625" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="54.33203125" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5546875" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.6640625" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5546875" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="21.33203125" collapsed="false"/>
+    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.42578125" customWidth="1"/>
+    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:20">
+    <row r="1" spans="1:20" ht="30">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>116</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>117</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
         <v>118</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
         <v>119</v>
       </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>120</v>
       </c>
-      <c r="I1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>121</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>122</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>124</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="P1" t="s">
         <v>125</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>126</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>128</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>129</v>
       </c>
-      <c r="S1" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" t="s">
-        <v>131</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="14.33203125" collapsed="false"/>
+    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>74</v>
@@ -1302,31 +1433,234 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07B9C67-F777-4764-8D3B-EBA0A42D75D1}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>149</v>
+      </c>
+      <c r="R1" t="s">
+        <v>150</v>
+      </c>
+      <c r="S1" t="s">
+        <v>151</v>
+      </c>
+      <c r="T1" t="s">
+        <v>152</v>
+      </c>
+      <c r="U1" t="s">
+        <v>153</v>
+      </c>
+      <c r="V1" t="s">
+        <v>154</v>
+      </c>
+      <c r="W1" t="s">
+        <v>155</v>
+      </c>
+      <c r="X1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2">
+        <v>9890324119</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" t="s">
+        <v>172</v>
+      </c>
+      <c r="S2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T2" t="s">
+        <v>174</v>
+      </c>
+      <c r="U2">
+        <v>500</v>
+      </c>
+      <c r="V2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>175</v>
+      </c>
+      <c r="X2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{5F876261-357A-4782-A972-98082BC9ED1B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE86E0-FEB9-4743-ADAF-C162F66B8CC3}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="28.8" r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1400,23 +1734,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.6640625" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1448,27 +1782,27 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.33203125" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1492,29 +1826,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="19.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.6640625" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1607,52 +1941,52 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AU1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.33203125" collapsed="true"/>
-    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
-    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.33203125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.33203125" collapsed="true"/>
-    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
-    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
-    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.6640625" collapsed="true"/>
-    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.33203125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.6640625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.6640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.44140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="65.33203125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
-    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.6640625" collapsed="true"/>
-    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.33203125" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.6640625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.6640625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.44140625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.44140625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.6640625" collapsed="true"/>
-    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="7" width="9" style="1" collapsed="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9" style="11" collapsed="1"/>
+    <col min="12" max="20" width="9" style="1" collapsed="1"/>
+    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="11" collapsed="1"/>
+    <col min="25" max="26" width="9" style="1" collapsed="1"/>
+    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -1796,22 +2130,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1887,21 +2221,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row customFormat="1" r="1" s="14" spans="1:3">
+    <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -1912,35 +2246,35 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.33203125" collapsed="true"/>
-    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1952,7 +2286,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push rahul excel again for missing
push rahul excel again for missing
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023E4A77-41E6-40E8-8684-B1FF821B9451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDF6E9D-CA92-4E4C-A145-C9761BCAC008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="WithdrawalAccount" sheetId="14" r:id="rId14"/>
     <sheet name="Order" sheetId="15" r:id="rId15"/>
     <sheet name="PrimeUser" sheetId="16" r:id="rId16"/>
+    <sheet name="CreditCardTestData" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="187">
   <si>
     <t>パスワード</t>
   </si>
@@ -590,6 +591,30 @@
   </si>
   <si>
     <t>TestPF1221_19082021181704</t>
+  </si>
+  <si>
+    <t>ValidCreditCardNumer</t>
+  </si>
+  <si>
+    <t>InValidCreditCardNumer</t>
+  </si>
+  <si>
+    <t>ExpirationMonth</t>
+  </si>
+  <si>
+    <t>ExpirationYear</t>
+  </si>
+  <si>
+    <t>CreditCardHolderName</t>
+  </si>
+  <si>
+    <t>SecurityCode</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>7月</t>
   </si>
 </sst>
 </file>
@@ -1614,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE86E0-FEB9-4743-ADAF-C162F66B8CC3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1640,6 +1665,64 @@
       </c>
       <c r="C2" t="s">
         <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B7C8F9-2D8B-47EC-A32F-DEA81E76B303}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="A2" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2025</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added methods for prime user
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDF6E9D-CA92-4E4C-A145-C9761BCAC008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="3343" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -32,6 +26,7 @@
     <sheet name="CreditCardTestData" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:Q9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -620,7 +615,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1104,17 +1099,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1136,23 +1131,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:9" ht="17.600000000000001">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1180,14 +1175,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.3046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1201,44 +1196,44 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.69140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.69140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.84375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.69140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.69140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.84375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.3828125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.69140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.3828125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.69140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1339,36 +1334,36 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.3828125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.3828125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.3828125" customWidth="1"/>
+    <col min="15" max="15" width="32.69140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.3046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.53515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="64.53515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row r="1" spans="1:20" ht="29.15">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1436,16 +1431,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1470,14 +1465,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07B9C67-F777-4764-8D3B-EBA0A42D75D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="14" t="s">
@@ -1629,21 +1624,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{5F876261-357A-4782-A972-98082BC9ED1B}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE86E0-FEB9-4743-ADAF-C162F66B8CC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="14" t="s">
@@ -1673,14 +1668,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B7C8F9-2D8B-47EC-A32F-DEA81E76B303}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="9" t="s">
@@ -1731,19 +1726,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row r="1" spans="1:12" ht="29.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1781,7 +1776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="29.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1822,17 +1817,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1870,21 +1865,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.3046875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1915,22 +1910,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2024,8 +2019,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2033,42 +2028,42 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="9" style="11" collapsed="1"/>
     <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" style="11" collapsed="1"/>
     <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="28" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.3046875" style="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2219,16 +2214,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.3046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2309,14 +2304,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
@@ -2347,16 +2342,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Revert "Sopan membership pt 60 & pt 61"
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sopan\Project\Automation\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDF6E9D-CA92-4E4C-A145-C9761BCAC008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="3540" windowWidth="17280" windowHeight="9420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -24,7 +25,11 @@
     <sheet name="Header" sheetId="10" r:id="rId10"/>
     <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
     <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
-    <sheet name="Sheet2" sheetId="13" r:id="rId13"/>
+    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
+    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId14"/>
+    <sheet name="Order" sheetId="15" r:id="rId15"/>
+    <sheet name="PrimeUser" sheetId="16" r:id="rId16"/>
+    <sheet name="CreditCardTestData" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="187">
   <si>
     <t>パスワード</t>
   </si>
@@ -315,15 +320,9 @@
     <t>プライム会員</t>
   </si>
   <si>
-    <t>TestPF1221+13082021092544@gmail.com</t>
-  </si>
-  <si>
     <t>pfqa_123</t>
   </si>
   <si>
-    <t>TestPF1221_13082021092544</t>
-  </si>
-  <si>
     <t>【スタギア 受験の窓口】各種検定・試験をお得に便利に申込み！</t>
   </si>
   <si>
@@ -450,25 +449,178 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>Freeuser</t>
-  </si>
-  <si>
-    <t>Primeuser</t>
-  </si>
-  <si>
-    <t>CASEC</t>
-  </si>
-  <si>
-    <t>漢検</t>
-  </si>
-  <si>
-    <t>Kanji Kentei</t>
+    <t>sahaj_automate</t>
+  </si>
+  <si>
+    <t>TestPF1221+17082021184752@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_17082021184752</t>
+  </si>
+  <si>
+    <t>expectedInvalidCreditCardText</t>
+  </si>
+  <si>
+    <t>expectedBlankCreditCardText</t>
+  </si>
+  <si>
+    <t>validConStoreKanjiName</t>
+  </si>
+  <si>
+    <t>validConStoreKanaName</t>
+  </si>
+  <si>
+    <t>validConStorePhoneno</t>
+  </si>
+  <si>
+    <t>validConStoreEmailAddress</t>
+  </si>
+  <si>
+    <t>InValidConStoreEmailAddress</t>
+  </si>
+  <si>
+    <t>expectedinvalidEmailConStoreText</t>
+  </si>
+  <si>
+    <t>expectedBlankConStoreText</t>
+  </si>
+  <si>
+    <t>expectedKanaConStoreText</t>
+  </si>
+  <si>
+    <t>expectedTelePhoneConStoreText</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageExpectedBuyAgainButton</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageExpectedStatusPaymentUnconfirmed</t>
+  </si>
+  <si>
+    <t>ThankYouPageThankYouForYourApplicationLabel</t>
+  </si>
+  <si>
+    <t>startNowButtonSTRStartNowButton</t>
+  </si>
+  <si>
+    <t>ThankYouPageThankYouForPrimeLabel</t>
+  </si>
+  <si>
+    <t>ThankYouPageTopPageButton</t>
+  </si>
+  <si>
+    <t>OrderHistoryPageStatusPaymentconfirmed</t>
+  </si>
+  <si>
+    <t>PrimeLabel</t>
+  </si>
+  <si>
+    <t>PrimePrice</t>
+  </si>
+  <si>
+    <t>PrimeButtonOnHeaderPage</t>
+  </si>
+  <si>
+    <t>MembershipPagePrimeCreditCardLabel</t>
+  </si>
+  <si>
+    <t>LearnButtonLabelForKankenProduct</t>
+  </si>
+  <si>
+    <t>ご利用いただけないクレジットカードです。</t>
+  </si>
+  <si>
+    <t>入力してください</t>
+  </si>
+  <si>
+    <t>柏木佳　奈子</t>
+  </si>
+  <si>
+    <t>カシワギ　カナコ</t>
+  </si>
+  <si>
+    <t>rahul.shinde+82@scispl.com</t>
+  </si>
+  <si>
+    <t>rahul.shinde</t>
+  </si>
+  <si>
+    <t>有効なメールアドレスを入力してください</t>
+  </si>
+  <si>
+    <t>氏名（漢字）を入力してください</t>
+  </si>
+  <si>
+    <t>氏名（カナ）を入力してください</t>
+  </si>
+  <si>
+    <t>電話番号を入力してください</t>
+  </si>
+  <si>
+    <t>再度購入</t>
+  </si>
+  <si>
+    <t>支払い未確認</t>
+  </si>
+  <si>
+    <t>ご購入ありがとうございます。</t>
+  </si>
+  <si>
+    <t>今すぐはじめる</t>
+  </si>
+  <si>
+    <t>ありがとうございます！</t>
+  </si>
+  <si>
+    <t>トップページ</t>
+  </si>
+  <si>
+    <t>支払い確認済み</t>
+  </si>
+  <si>
+    <t>プライム会員プラン</t>
+  </si>
+  <si>
+    <t>クレジットカード支払い</t>
+  </si>
+  <si>
+    <t>近日公開</t>
+  </si>
+  <si>
+    <t>TestPF1221+19082021181704@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_19082021181704</t>
+  </si>
+  <si>
+    <t>ValidCreditCardNumer</t>
+  </si>
+  <si>
+    <t>InValidCreditCardNumer</t>
+  </si>
+  <si>
+    <t>ExpirationMonth</t>
+  </si>
+  <si>
+    <t>ExpirationYear</t>
+  </si>
+  <si>
+    <t>CreditCardHolderName</t>
+  </si>
+  <si>
+    <t>SecurityCode</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>7月</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -586,7 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -637,6 +789,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,7 +851,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -750,7 +903,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -951,11 +1104,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -967,7 +1120,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>74</v>
@@ -983,14 +1136,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1001,22 +1154,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18">
       <c r="A1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="G1" s="19"/>
       <c r="I1" s="20"/>
@@ -1027,7 +1180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1039,7 +1192,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1048,7 +1201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -1090,94 +1243,94 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" t="s">
         <v>107</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" t="s">
+        <v>99</v>
+      </c>
+      <c r="X1" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" t="s">
-        <v>112</v>
-      </c>
-      <c r="U1" t="s">
-        <v>113</v>
-      </c>
-      <c r="V1" t="s">
-        <v>114</v>
-      </c>
-      <c r="W1" t="s">
-        <v>101</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>101</v>
-      </c>
       <c r="AB1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD1" t="s">
         <v>98</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1186,7 +1339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1217,64 +1370,359 @@
   <sheetData>
     <row r="1" spans="1:20" ht="30">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
         <v>115</v>
       </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07B9C67-F777-4764-8D3B-EBA0A42D75D1}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="H1" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="I1" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="K1" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="L1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>149</v>
+      </c>
+      <c r="R1" t="s">
+        <v>150</v>
+      </c>
+      <c r="S1" t="s">
+        <v>151</v>
+      </c>
+      <c r="T1" t="s">
+        <v>152</v>
+      </c>
+      <c r="U1" t="s">
+        <v>153</v>
+      </c>
+      <c r="V1" t="s">
+        <v>154</v>
+      </c>
+      <c r="W1" t="s">
+        <v>155</v>
+      </c>
+      <c r="X1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2">
+        <v>9890324119</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" t="s">
+        <v>172</v>
+      </c>
+      <c r="S2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T2" t="s">
+        <v>174</v>
+      </c>
+      <c r="U2">
+        <v>500</v>
+      </c>
+      <c r="V2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" t="s">
+        <v>175</v>
+      </c>
+      <c r="X2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{5F876261-357A-4782-A972-98082BC9ED1B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE86E0-FEB9-4743-ADAF-C162F66B8CC3}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B7C8F9-2D8B-47EC-A32F-DEA81E76B303}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="A2" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2025</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2">
         <v>123</v>
       </c>
-      <c r="M1" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R1" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" t="s">
-        <v>131</v>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1283,7 +1731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1374,7 +1822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1422,7 +1870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1467,7 +1915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1576,8 +2024,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1585,7 +2033,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
@@ -1771,7 +2219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1861,7 +2309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1883,13 +2331,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1899,48 +2347,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9" style="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle product list dynamic xpath
handle product list dynamic xpath
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,39 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDF6E9D-CA92-4E4C-A145-C9761BCAC008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{36EEEACC-7462-40B9-AD25-D9239D7C7025}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="17" firstSheet="13" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
-    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
-    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
-    <sheet name="Header" sheetId="10" r:id="rId10"/>
-    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
-    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
-    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
-    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId14"/>
-    <sheet name="Order" sheetId="15" r:id="rId15"/>
-    <sheet name="PrimeUser" sheetId="16" r:id="rId16"/>
-    <sheet name="CreditCardTestData" sheetId="17" r:id="rId17"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
+    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
+    <sheet name="Header" r:id="rId10" sheetId="10"/>
+    <sheet name="MemberPlanAssert" r:id="rId11" sheetId="11"/>
+    <sheet name="FooterAssert" r:id="rId12" sheetId="12"/>
+    <sheet name="FooterTermsAssert" r:id="rId13" sheetId="13"/>
+    <sheet name="WithdrawalAccount" r:id="rId14" sheetId="14"/>
+    <sheet name="Order" r:id="rId15" sheetId="15"/>
+    <sheet name="PrimeUser" r:id="rId16" sheetId="16"/>
+    <sheet name="CreditCardTestData" r:id="rId17" sheetId="17"/>
+    <sheet name="ProductForOrder" r:id="rId18" sheetId="18"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="193">
   <si>
     <t>パスワード</t>
   </si>
@@ -452,12 +453,6 @@
     <t>sahaj_automate</t>
   </si>
   <si>
-    <t>TestPF1221+17082021184752@gmail.com</t>
-  </si>
-  <si>
-    <t>TestPF1221_17082021184752</t>
-  </si>
-  <si>
     <t>expectedInvalidCreditCardText</t>
   </si>
   <si>
@@ -587,12 +582,6 @@
     <t>近日公開</t>
   </si>
   <si>
-    <t>TestPF1221+19082021181704@gmail.com</t>
-  </si>
-  <si>
-    <t>TestPF1221_19082021181704</t>
-  </si>
-  <si>
     <t>ValidCreditCardNumer</t>
   </si>
   <si>
@@ -615,12 +604,43 @@
   </si>
   <si>
     <t>7月</t>
+  </si>
+  <si>
+    <t>TestPF1221+20082021154359@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_20082021154359</t>
+  </si>
+  <si>
+    <t>ProductCategory</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>漢検</t>
+  </si>
+  <si>
+    <t>スタギア漢検３級プレミアム６ヶ月</t>
+  </si>
+  <si>
+    <t>TestPF1221+23082021184147@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_23082021184147</t>
+  </si>
+  <si>
+    <t>TestPF1221+23082021184937@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_23082021184937</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -735,68 +755,68 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -813,10 +833,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -851,7 +871,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -903,7 +923,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1014,21 +1034,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1045,7 +1065,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1097,15 +1117,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -1113,9 +1133,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1136,15 +1156,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -1152,7 +1172,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row ht="18" r="1" spans="1:9">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1175,19 +1195,19 @@
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1196,13 +1216,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
-  <dimension ref="A1:AD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471D0663-8EA0-43F1-BDB6-4204A5537BD0}">
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -1210,35 +1230,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="99.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="57.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="53.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="58.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="49.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1334,13 +1354,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AD7D05-3566-447E-A6B3-E609BBDAA995}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1348,27 +1368,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="53.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="92.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row ht="30" r="1" spans="1:20">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1431,13 +1451,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564AC067-E671-4DB1-A34F-9AAA68AFB8FE}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1445,7 +1465,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1465,13 +1485,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07B9C67-F777-4764-8D3B-EBA0A42D75D1}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07B9C67-F777-4764-8D3B-EBA0A42D75D1}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
@@ -1484,73 +1504,73 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
         <v>134</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>135</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>136</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>137</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>140</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>141</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>142</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>143</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>144</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>145</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>146</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>147</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>149</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>150</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>151</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>152</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>153</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>154</v>
-      </c>
-      <c r="W1" t="s">
-        <v>155</v>
-      </c>
-      <c r="X1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -1558,61 +1578,61 @@
         <v>68</v>
       </c>
       <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
         <v>157</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>158</v>
-      </c>
-      <c r="D2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" t="s">
-        <v>160</v>
       </c>
       <c r="F2">
         <v>9890324119</v>
       </c>
       <c r="G2" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" t="s">
         <v>161</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>162</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>163</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>164</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>165</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>166</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>167</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>168</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>169</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>170</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>171</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>172</v>
-      </c>
-      <c r="S2" t="s">
-        <v>173</v>
-      </c>
-      <c r="T2" t="s">
-        <v>174</v>
       </c>
       <c r="U2">
         <v>500</v>
@@ -1621,23 +1641,65 @@
         <v>87</v>
       </c>
       <c r="W2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="X2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{5F876261-357A-4782-A972-98082BC9ED1B}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{5F876261-357A-4782-A972-98082BC9ED1B}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE86E0-FEB9-4743-ADAF-C162F66B8CC3}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FE86E0-FEB9-4743-ADAF-C162F66B8CC3}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B7C8F9-2D8B-47EC-A32F-DEA81E76B303}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -1645,94 +1707,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row customFormat="1" r="1" s="1" spans="1:7">
+      <c r="A1" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D1" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="E1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="1" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2025</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B7C8F9-2D8B-47EC-A32F-DEA81E76B303}">
-  <dimension ref="A1:G2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC204D93-2F00-4B5A-993F-989F5FDE1BDF}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
-      <c r="A1" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B1" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="1">
-        <v>2025</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2">
-        <v>123</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -1740,10 +1800,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row ht="30" r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1781,7 +1841,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row ht="30" r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1817,13 +1877,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1831,9 +1891,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1865,13 +1925,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1879,13 +1939,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1909,14 +1969,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1924,14 +1984,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2024,17 +2084,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -2042,34 +2102,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9" style="11" collapsed="1"/>
-    <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="11" collapsed="1"/>
-    <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.7109375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -2213,14 +2273,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
@@ -2228,7 +2288,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2304,21 +2364,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1">
+    <row customFormat="1" r="1" s="14" spans="1:3">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -2329,26 +2394,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -2356,8 +2421,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2369,7 +2434,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push product category and name for rahul
push product category and name for rahul
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sopan\Project\Automation\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A07870-FDE2-4137-A543-E1FC0893787F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -21,14 +22,15 @@
     <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
     <sheet name="NewUser" sheetId="8" r:id="rId8"/>
     <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
-    <sheet name="Header" sheetId="10" r:id="rId10"/>
-    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId11"/>
-    <sheet name="FooterAssert" sheetId="12" r:id="rId12"/>
-    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId13"/>
-    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId14"/>
-    <sheet name="Order" sheetId="15" r:id="rId15"/>
-    <sheet name="PrimeUser" sheetId="16" r:id="rId16"/>
-    <sheet name="CreditCardTestData" sheetId="17" r:id="rId17"/>
+    <sheet name="ProductForOrder" sheetId="18" r:id="rId10"/>
+    <sheet name="Header" sheetId="10" r:id="rId11"/>
+    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId12"/>
+    <sheet name="FooterAssert" sheetId="12" r:id="rId13"/>
+    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId14"/>
+    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId15"/>
+    <sheet name="Order" sheetId="15" r:id="rId16"/>
+    <sheet name="PrimeUser" sheetId="16" r:id="rId17"/>
+    <sheet name="CreditCardTestData" sheetId="17" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="195">
   <si>
     <t>パスワード</t>
   </si>
@@ -630,11 +632,20 @@
   <si>
     <t>漢検</t>
   </si>
+  <si>
+    <t>ProductCategory</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>スタギア漢検３級プレミアム６ヶ月</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1118,7 +1129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1150,14 +1161,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D47865B-8A6C-4783-879E-D9D8ECC29015}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1193,8 +1235,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1214,8 +1256,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -1352,8 +1394,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1449,8 +1491,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1483,8 +1525,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1643,14 +1685,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1686,8 +1728,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1745,7 +1787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1836,7 +1878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1884,7 +1926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1929,7 +1971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2038,8 +2080,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2047,7 +2089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
@@ -2233,7 +2275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2323,7 +2365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2361,10 +2403,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
study gear link working
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,40 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A07870-FDE2-4137-A543-E1FC0893787F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{60A07870-FDE2-4137-A543-E1FC0893787F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="9" firstSheet="6" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
-    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
-    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
-    <sheet name="ProductForOrder" sheetId="18" r:id="rId10"/>
-    <sheet name="Header" sheetId="10" r:id="rId11"/>
-    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId12"/>
-    <sheet name="FooterAssert" sheetId="12" r:id="rId13"/>
-    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId14"/>
-    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId15"/>
-    <sheet name="Order" sheetId="15" r:id="rId16"/>
-    <sheet name="PrimeUser" sheetId="16" r:id="rId17"/>
-    <sheet name="CreditCardTestData" sheetId="17" r:id="rId18"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
+    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
+    <sheet name="ProductForOrder" r:id="rId10" sheetId="18"/>
+    <sheet name="Header" r:id="rId11" sheetId="10"/>
+    <sheet name="MemberPlanAssert" r:id="rId12" sheetId="11"/>
+    <sheet name="FooterAssert" r:id="rId13" sheetId="12"/>
+    <sheet name="FooterTermsAssert" r:id="rId14" sheetId="13"/>
+    <sheet name="WithdrawalAccount" r:id="rId15" sheetId="14"/>
+    <sheet name="Order" r:id="rId16" sheetId="15"/>
+    <sheet name="PrimeUser" r:id="rId17" sheetId="16"/>
+    <sheet name="CreditCardTestData" r:id="rId18" sheetId="17"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="197">
   <si>
     <t>パスワード</t>
   </si>
@@ -641,11 +641,18 @@
   <si>
     <t>スタギア漢検３級プレミアム６ヶ月</t>
   </si>
+  <si>
+    <t>TestPF1221+24082021105359@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_24082021105359</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -760,68 +767,68 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -838,10 +845,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -876,7 +883,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -928,7 +935,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1039,21 +1046,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1070,7 +1077,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1122,15 +1129,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -1138,9 +1145,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1161,15 +1168,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D47865B-8A6C-4783-879E-D9D8ECC29015}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D47865B-8A6C-4783-879E-D9D8ECC29015}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B2"/>
@@ -1194,13 +1201,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -1208,7 +1215,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row ht="18" r="1" spans="1:9">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1231,19 +1238,19 @@
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1252,13 +1259,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:AD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -1266,35 +1273,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="42.7109375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="99.85546875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="57.28515625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="53.85546875" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="58.7109375" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="60.7109375" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="49.7109375" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.85546875" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="35.28515625" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="24.85546875" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.7109375" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1390,13 +1397,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1404,27 +1411,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="53.42578125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5703125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.28515625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.42578125" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5703125" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.140625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="92.140625" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="41.42578125" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="32.7109375" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="54.28515625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5703125" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5703125" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row ht="30" r="1" spans="1:20">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1487,13 +1494,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1501,7 +1508,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1521,13 +1528,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
@@ -1685,15 +1692,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -1724,13 +1731,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -1738,7 +1745,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row customFormat="1" r="1" s="1" spans="1:7">
       <c r="A1" s="9" t="s">
         <v>179</v>
       </c>
@@ -1758,7 +1765,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+    <row customFormat="1" r="2" s="1" spans="1:7">
       <c r="A2" s="10" t="s">
         <v>185</v>
       </c>
@@ -1782,13 +1789,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -1796,10 +1803,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row ht="30" r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1837,7 +1844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row ht="30" r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1873,13 +1880,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1887,9 +1894,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1921,13 +1928,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1935,13 +1942,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1965,14 +1972,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1980,14 +1987,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2080,17 +2087,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -2098,34 +2105,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9" style="11" collapsed="1"/>
-    <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="11" collapsed="1"/>
-    <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.7109375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -2269,14 +2276,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
@@ -2284,7 +2291,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2360,13 +2367,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -2374,7 +2381,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1">
+    <row customFormat="1" r="1" s="14" spans="1:3">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -2385,26 +2392,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -2412,10 +2419,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2447,7 +2454,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data for delete mail
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,40 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFE20DD-6439-4237-A285-1BDC244BD47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{ABFE20DD-6439-4237-A285-1BDC244BD47A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="9" firstSheet="6" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="5" r:id="rId1"/>
-    <sheet name="Register" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
-    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
-    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
-    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
-    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
-    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
-    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
-    <sheet name="ProductForOrder" sheetId="18" r:id="rId10"/>
-    <sheet name="Header" sheetId="10" r:id="rId11"/>
-    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId12"/>
-    <sheet name="FooterAssert" sheetId="12" r:id="rId13"/>
-    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId14"/>
-    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId15"/>
-    <sheet name="Order" sheetId="15" r:id="rId16"/>
-    <sheet name="PrimeUser" sheetId="16" r:id="rId17"/>
-    <sheet name="CreditCardTestData" sheetId="17" r:id="rId18"/>
+    <sheet name="User" r:id="rId1" sheetId="5"/>
+    <sheet name="Register" r:id="rId2" sheetId="1"/>
+    <sheet name="Product" r:id="rId3" sheetId="2"/>
+    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
+    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
+    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
+    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
+    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
+    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
+    <sheet name="ProductForOrder" r:id="rId10" sheetId="18"/>
+    <sheet name="Header" r:id="rId11" sheetId="10"/>
+    <sheet name="MemberPlanAssert" r:id="rId12" sheetId="11"/>
+    <sheet name="FooterAssert" r:id="rId13" sheetId="12"/>
+    <sheet name="FooterTermsAssert" r:id="rId14" sheetId="13"/>
+    <sheet name="WithdrawalAccount" r:id="rId15" sheetId="14"/>
+    <sheet name="Order" r:id="rId16" sheetId="15"/>
+    <sheet name="PrimeUser" r:id="rId17" sheetId="16"/>
+    <sheet name="CreditCardTestData" r:id="rId18" sheetId="17"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="201">
   <si>
     <t>パスワード</t>
   </si>
@@ -641,11 +641,30 @@
   <si>
     <t>スタギア漢検３級プレミアム６ヶ月</t>
   </si>
+  <si>
+    <t>TestPF1221+26082021113340@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_26082021113340</t>
+  </si>
+  <si>
+    <t>TestPF1221+26082021130353@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_26082021130353</t>
+  </si>
+  <si>
+    <t>TestPF1221+26082021133822@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPF1221_26082021133822</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -760,68 +779,68 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -838,10 +857,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -876,7 +895,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -928,7 +947,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1039,21 +1058,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1070,7 +1089,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1122,15 +1141,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -1138,9 +1157,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1161,15 +1180,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
@@ -1194,13 +1213,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -1208,7 +1227,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row ht="18" r="1" spans="1:9">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1231,19 +1250,19 @@
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1252,13 +1271,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -1266,35 +1285,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="99.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="57.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="53.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="58.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="60.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="49.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1390,13 +1409,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1404,27 +1423,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="53.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="80.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="92.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="44.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="64.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row ht="30" r="1" spans="1:20">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1487,13 +1506,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1501,7 +1520,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1521,13 +1540,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
@@ -1685,15 +1704,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -1724,13 +1743,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -1738,7 +1757,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row customFormat="1" r="1" s="1" spans="1:7">
       <c r="A1" s="9" t="s">
         <v>179</v>
       </c>
@@ -1758,7 +1777,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+    <row customFormat="1" r="2" s="1" spans="1:7">
       <c r="A2" s="10" t="s">
         <v>185</v>
       </c>
@@ -1782,13 +1801,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -1796,10 +1815,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row ht="30" r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1837,7 +1856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row ht="30" r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1873,13 +1892,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1887,9 +1906,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1921,13 +1940,13 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1935,13 +1954,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.28515625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1965,14 +1984,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1980,14 +1999,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
+    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2080,17 +2099,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AT1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
@@ -2098,34 +2117,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9" style="11" collapsed="1"/>
-    <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="11" collapsed="1"/>
-    <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
+    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
+    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
+    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.7109375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="65.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -2269,14 +2288,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
@@ -2284,7 +2303,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2360,13 +2379,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -2374,7 +2393,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1">
+    <row customFormat="1" r="1" s="14" spans="1:3">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -2385,26 +2404,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2412,10 +2431,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2447,7 +2466,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed string in sheet and reference
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\WorkSpace\Project\Workspace\GitPFAutomation\PlatformTesting\platform\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFE20DD-6439-4237-A285-1BDC244BD47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20734" windowHeight="11160" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="5" r:id="rId1"/>
@@ -645,7 +644,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1129,17 +1128,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1161,21 +1160,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1199,16 +1198,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:9" ht="17.600000000000001">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1236,14 +1235,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.3046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1257,44 +1256,44 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.69140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.69140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.84375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.69140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.69140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.84375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.3828125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.69140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.3828125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.69140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1395,36 +1394,36 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.3828125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.3828125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.15234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.3828125" customWidth="1"/>
+    <col min="15" max="15" width="32.69140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.3046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.53515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="64.53515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30">
+    <row r="1" spans="1:20" ht="29.15">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1492,16 +1491,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1526,14 +1525,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="14" t="s">
@@ -1685,21 +1684,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="14" t="s">
@@ -1729,14 +1728,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="9" t="s">
@@ -1787,19 +1786,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row r="1" spans="1:12" ht="29.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="29.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1878,17 +1877,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1926,21 +1925,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.3046875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1971,22 +1970,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2080,8 +2079,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2089,42 +2088,42 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="7" width="9" style="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="9" style="11" collapsed="1"/>
     <col min="12" max="20" width="9" style="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" style="11" collapsed="1"/>
     <col min="25" max="26" width="9" style="1" collapsed="1"/>
-    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="28" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.3046875" style="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2275,16 +2274,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.3046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2365,14 +2364,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
@@ -2403,18 +2402,18 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated sheet as per main
</commit_message>
<xml_diff>
--- a/platform/TestData/NewTestData.xlsx
+++ b/platform/TestData/NewTestData.xlsx
@@ -1,34 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\PlatformTesting\platform\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFE20DD-6439-4237-A285-1BDC244BD47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="6" windowHeight="3343" windowWidth="17760" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User" r:id="rId1" sheetId="5"/>
-    <sheet name="Register" r:id="rId2" sheetId="1"/>
-    <sheet name="Product" r:id="rId3" sheetId="2"/>
-    <sheet name="CCPayment" r:id="rId4" sheetId="3"/>
-    <sheet name="ConvenienceStorePayment" r:id="rId5" sheetId="4"/>
-    <sheet name="UpdateAccountInformation" r:id="rId6" sheetId="6"/>
-    <sheet name="ValidationStrings" r:id="rId7" sheetId="7"/>
-    <sheet name="NewUser" r:id="rId8" sheetId="8"/>
-    <sheet name="MembershipStatus" r:id="rId9" sheetId="9"/>
-    <sheet name="Header" r:id="rId10" sheetId="10"/>
-    <sheet name="MemberPlanAssert" r:id="rId11" sheetId="11"/>
-    <sheet name="FooterAssert" r:id="rId12" sheetId="12"/>
-    <sheet name="FooterTermsAssert" r:id="rId13" sheetId="13"/>
-    <sheet name="WithdrawalAccount" r:id="rId14" sheetId="14"/>
-    <sheet name="Order" r:id="rId15" sheetId="15"/>
-    <sheet name="PrimeUser" r:id="rId16" sheetId="16"/>
-    <sheet name="CreditCardTestData" r:id="rId17" sheetId="17"/>
+    <sheet name="User" sheetId="5" r:id="rId1"/>
+    <sheet name="Register" sheetId="1" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" r:id="rId3"/>
+    <sheet name="CCPayment" sheetId="3" r:id="rId4"/>
+    <sheet name="ConvenienceStorePayment" sheetId="4" r:id="rId5"/>
+    <sheet name="UpdateAccountInformation" sheetId="6" r:id="rId6"/>
+    <sheet name="ValidationStrings" sheetId="7" r:id="rId7"/>
+    <sheet name="NewUser" sheetId="8" r:id="rId8"/>
+    <sheet name="MembershipStatus" sheetId="9" r:id="rId9"/>
+    <sheet name="ProductForOrder" sheetId="18" r:id="rId10"/>
+    <sheet name="Header" sheetId="10" r:id="rId11"/>
+    <sheet name="MemberPlanAssert" sheetId="11" r:id="rId12"/>
+    <sheet name="FooterAssert" sheetId="12" r:id="rId13"/>
+    <sheet name="FooterTermsAssert" sheetId="13" r:id="rId14"/>
+    <sheet name="WithdrawalAccount" sheetId="14" r:id="rId15"/>
+    <sheet name="Order" sheetId="15" r:id="rId16"/>
+    <sheet name="PrimeUser" sheetId="16" r:id="rId17"/>
+    <sheet name="CreditCardTestData" sheetId="17" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R9"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="195">
   <si>
     <t>パスワード</t>
   </si>
@@ -612,17 +618,34 @@
     <t>7月</t>
   </si>
   <si>
-    <t>TestPF1221+23082021090946@gmail.com</t>
-  </si>
-  <si>
-    <t>TestPF1221_23082021090946</t>
+    <t>Freeuser</t>
+  </si>
+  <si>
+    <t>Primeuser</t>
+  </si>
+  <si>
+    <t>CASEC</t>
+  </si>
+  <si>
+    <t>Kanji Kentei</t>
+  </si>
+  <si>
+    <t>漢検</t>
+  </si>
+  <si>
+    <t>ProductCategory</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>スタギア漢検３級プレミアム６ヶ月</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -737,68 +760,68 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -815,10 +838,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -853,7 +876,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -905,7 +928,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1016,21 +1039,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1047,7 +1070,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1099,25 +1122,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.3046875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.69140625" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1138,23 +1161,54 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="merabafo@livinginsurance.co.uk" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="merabafo@livinginsurance.co.uk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row ht="17.600000000000001" r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="16" t="s">
         <v>89</v>
       </c>
@@ -1177,19 +1231,19 @@
       <c r="I1" s="20"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.3046875" collapsed="false"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1198,49 +1252,49 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE1"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.69140625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.84375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.3828125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="60.69140625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="42.69140625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="99.84375" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="57.3046875" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="60.69140625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="53.84375" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="58.0" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="58.69140625" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="60.69140625" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="49.69140625" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="18.69140625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="24.84375" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="35.3046875" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="24.84375" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="29.0" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="20.69140625" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.69140625" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="25.3828125" collapsed="false"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="18.69140625" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="22.84375" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="25.3828125" collapsed="false"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="18.69140625" collapsed="false"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.84375" collapsed="false"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="54" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="54" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -1336,41 +1390,41 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.3046875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="53.3828125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.53515625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="48.3046875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="35.3828125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.3828125" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="80.53515625" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="25.15234375" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="92.15234375" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="41.3828125" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="32.69140625" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="54.3046875" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="44.53515625" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.69140625" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="64.53515625" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="21.3046875" collapsed="false"/>
+    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.42578125" customWidth="1"/>
+    <col min="15" max="15" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="29.15" r="1" spans="1:20">
+    <row r="1" spans="1:20" ht="30">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1433,21 +1487,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="14.3046875" collapsed="false"/>
+    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1467,19 +1521,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="14" t="s">
@@ -1631,21 +1685,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="14" t="s">
@@ -1670,21 +1724,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:7">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>179</v>
       </c>
@@ -1704,7 +1758,7 @@
         <v>184</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:7">
+    <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>185</v>
       </c>
@@ -1728,24 +1782,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29.15" r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="29.15" r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1819,23 +1873,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="23.3046875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.69140625" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1867,27 +1921,27 @@
       <c r="H3" s="4"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="17.3046875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.3828125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.3046875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.69140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.3046875" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1911,29 +1965,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="12.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="25.69140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="19.3828125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.3046875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="22.69140625" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2026,52 +2080,52 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
-    <hyperlink display="spoan.patil@scispl.com" r:id="rId2" ref="E3:E5"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3:E5" r:id="rId2" display="spoan.patil@scispl.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" style="1" width="9.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.3046875" collapsed="true"/>
-    <col min="11" max="11" style="11" width="9.0" collapsed="true"/>
-    <col min="12" max="20" style="1" width="9.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="20.3046875" collapsed="true"/>
-    <col min="24" max="24" style="11" width="9.0" collapsed="true"/>
-    <col min="25" max="26" style="1" width="9.0" collapsed="true"/>
-    <col min="27" max="28" bestFit="true" customWidth="true" style="1" width="52.69140625" collapsed="true"/>
-    <col min="29" max="30" bestFit="true" customWidth="true" style="1" width="75.3046875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="35.0" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="39.69140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="52.69140625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="51.3828125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="67.0" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="1" width="65.3046875" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
-    <col min="38" max="39" bestFit="true" customWidth="true" style="1" width="40.69140625" collapsed="true"/>
-    <col min="40" max="41" bestFit="true" customWidth="true" style="1" width="43.3046875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="33.69140625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="40.69140625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="38.3828125" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="45.3828125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="33.69140625" collapsed="true"/>
-    <col min="47" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="7" width="9" style="1" collapsed="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9" style="11" collapsed="1"/>
+    <col min="12" max="20" width="9" style="1" collapsed="1"/>
+    <col min="21" max="21" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="11" collapsed="1"/>
+    <col min="25" max="26" width="9" style="1" collapsed="1"/>
+    <col min="27" max="28" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="75.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="39.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="52.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="51.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="67" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="65.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="43.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="40.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="38.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="45.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="33.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -2215,22 +2269,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.3046875" collapsed="true"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2306,21 +2360,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row customFormat="1" r="1" s="14" spans="1:3">
+    <row r="1" spans="1:3" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>73</v>
       </c>
@@ -2331,47 +2385,69 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.3046875" collapsed="true"/>
-    <col min="2" max="16384" style="1" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>